<commit_message>
add for multicast locale
</commit_message>
<xml_diff>
--- a/archon/locale.xlsx
+++ b/archon/locale.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyungsok/Dev/archon_mcast/archon/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="29120" windowHeight="14940"/>
   </bookViews>
   <sheets>
     <sheet name="locale" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="74">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -262,6 +275,30 @@
   </si>
   <si>
     <t>개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group_Address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multicast Group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멀티캐스트 그룹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HWByteCnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW Byte Count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW 바이트 수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -309,16 +346,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -342,7 +379,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="기본" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -403,9 +440,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -438,9 +475,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -644,20 +681,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="3" customWidth="1"/>
-    <col min="2" max="4" width="25.625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="4"/>
+    <col min="1" max="1" width="25.6640625" style="3" customWidth="1"/>
+    <col min="2" max="4" width="25.6640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -671,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -685,7 +722,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
@@ -699,7 +736,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>66</v>
       </c>
@@ -713,7 +750,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -727,7 +764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -741,7 +778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -755,7 +792,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>58</v>
       </c>
@@ -769,7 +806,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -783,7 +820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -797,7 +834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -811,7 +848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>36</v>
       </c>
@@ -825,7 +862,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>21</v>
       </c>
@@ -839,7 +876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>40</v>
       </c>
@@ -853,7 +890,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -867,7 +904,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>38</v>
       </c>
@@ -881,7 +918,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -895,7 +932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -909,7 +946,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
@@ -923,7 +960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -937,7 +974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -951,7 +988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>60</v>
       </c>
@@ -965,7 +1002,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -979,7 +1016,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>62</v>
       </c>
@@ -993,7 +1030,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>56</v>
       </c>
@@ -1007,7 +1044,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>49</v>
       </c>
@@ -1021,7 +1058,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>47</v>
       </c>
@@ -1035,7 +1072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>64</v>
       </c>
@@ -1049,7 +1086,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
@@ -1063,7 +1100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>28</v>
       </c>
@@ -1077,7 +1114,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>30</v>
       </c>
@@ -1091,7 +1128,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>50</v>
       </c>
@@ -1105,7 +1142,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>32</v>
       </c>
@@ -1117,6 +1154,34 @@
       </c>
       <c r="D33" s="11" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>